<commit_message>
working on Goal Manager
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,68 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Estimated Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realized Time </t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Goal1</t>
+  </si>
+  <si>
+    <t>Task1.1</t>
+  </si>
+  <si>
+    <t>Task1.2</t>
+  </si>
+  <si>
+    <t>Task1.n</t>
+  </si>
+  <si>
+    <t>Goal2</t>
+  </si>
+  <si>
+    <t>Task2.1</t>
+  </si>
+  <si>
+    <t>Task2.2</t>
+  </si>
+  <si>
+    <t>Task2.n</t>
+  </si>
+  <si>
+    <t>Estimated Date</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>&lt;computed&gt;</t>
+  </si>
+  <si>
+    <t>(cons)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,14 +103,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +202,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +410,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add mvn-depend -> apache poi pentru Excel. Merge. Acm incerc sa deschid ambele frame-uri si sa comut intre ele
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="StandApp" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Description</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>(cons)</t>
+  </si>
+  <si>
+    <t>I will make StandApp in 2 months</t>
   </si>
 </sst>
 </file>
@@ -103,9 +106,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -413,39 +417,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="4" max="5" width="17.77734375" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="3"/>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -526,11 +531,16 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
am reusit sa fac scrierea unui goal in excel
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -71,12 +71,36 @@
   </si>
   <si>
     <t>I will make StandApp in 2 months</t>
+  </si>
+  <si>
+    <t>do the view</t>
+  </si>
+  <si>
+    <t>do the model</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,11 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,19 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -540,21 +566,119 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
+      <c r="B11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="n">
+        <v>44236.44610025463</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="n">
+        <v>44245.44610025463</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="n">
+        <v>44237.448924537035</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="n" s="4">
+        <v>44236.456396574074</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functioneaza comutarea AddGoal / EditGoal. lucrez la EditGoal
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>0%</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
 </sst>
 </file>
@@ -99,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -130,12 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A19" sqref="A19:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="1" max="1" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -499,8 +495,8 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
+      <c r="C3" s="2">
+        <v>44236.456396574074</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -522,8 +518,8 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
+      <c r="C4" s="2">
+        <v>44236.456396574074</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -542,16 +538,28 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="C5" s="2">
+        <v>44236.456396574074</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="2">
+        <v>44236.456396574074</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="2">
+        <v>44236.456396574074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -560,7 +568,9 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>44236.456396574074</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -569,7 +579,9 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>44236.456396574074</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -578,26 +590,41 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
+      <c r="C11" s="2">
+        <v>44236.456396574074</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
+      <c r="C13" s="2">
+        <v>44236.456396574074</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="C14" s="2">
+        <v>44236.456396574074</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="n">
-        <v>44236.44610025463</v>
+      <c r="C16" s="2">
+        <v>44236.456396574074</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -608,19 +635,22 @@
       <c r="F16" t="s">
         <v>24</v>
       </c>
-      <c r="G16" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="n">
-        <v>44245.44610025463</v>
+      <c r="C18" s="2">
+        <v>44236.456396574074</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
@@ -631,54 +661,8 @@
       <c r="F18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="n">
-        <v>44237.448924537035</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="n" s="4">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.0</v>
+      <c r="G18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
am lucrat la EDIT GOAL. trebuie sa fac partea de Add/Rmv Task
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>0%</t>
+  </si>
+  <si>
+    <t>FINISH</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD28"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,80 +598,89 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44236.456396574074</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>44236.456396574074</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2">
-        <v>44236.456396574074</v>
-      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="2"/>
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44236.456396574074</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" s="2">
+        <v>44236.456396574074</v>
+      </c>
+      <c r="D17" t="s">
         <v>23</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>24</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-    </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
+      <c r="A18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
functioneaza cum trebuie citirea / scrierea goalurilor EXCEL
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -28,21 +28,6 @@
     <t>Progress</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Goal1</t>
-  </si>
-  <si>
-    <t>Task1.1</t>
-  </si>
-  <si>
-    <t>Task1.2</t>
-  </si>
-  <si>
-    <t>Task1.n</t>
-  </si>
-  <si>
     <t>Goal2</t>
   </si>
   <si>
@@ -64,12 +49,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>&lt;computed&gt;</t>
-  </si>
-  <si>
-    <t>(cons)</t>
-  </si>
-  <si>
     <t>I will make StandApp in 2 months</t>
   </si>
   <si>
@@ -85,21 +64,40 @@
     <t>description</t>
   </si>
   <si>
-    <t>00:00</t>
-  </si>
-  <si>
     <t>0%</t>
   </si>
   <si>
-    <t>FINISH</t>
+    <t>fafsafa</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abc2</t>
+  </si>
+  <si>
+    <t>VREAU SA FIU ARTIST</t>
+  </si>
+  <si>
+    <t>0|0</t>
+  </si>
+  <si>
+    <t>finish this damn app</t>
+  </si>
+  <si>
+    <t>brandNewGoal -&gt; IULI CONDUCE LUMEEEEA</t>
+  </si>
+  <si>
+    <t>Just Started</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/MM/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,11 +134,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,44 +449,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A13" sqref="A13:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="8"/>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -485,202 +495,239 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
+      <c r="A3" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
-        <v>44236.456396574074</v>
+        <v>44241.456400462965</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2">
-        <v>44236.456396574074</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="6">
+        <v>44238.456400462965</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2">
-        <v>44236.456396574074</v>
+        <v>44239.456400462965</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>44236.456396574074</v>
       </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>44236.456396574074</v>
       </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44236.456396574074</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2">
-        <v>44236.456396574074</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44237.647051111111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2">
-        <v>44236.456396574074</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="4">
+        <v>44238.650255671295</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2">
-        <v>44236.456396574074</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="5">
+        <v>44239.650395219905</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2">
-        <v>44236.456396574074</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6">
+        <v>44247.652703865744</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2">
-        <v>44236.456396574074</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="C13" t="n" s="9">
+        <v>44237.72078783565</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
         <v>24</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
functioneaza citirea + Task &scrierea goalurilor -> lucrez la scrierea taskurilor
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -70,9 +70,6 @@
     <t>fafsafa</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>abc2</t>
   </si>
   <si>
@@ -89,15 +86,20 @@
   </si>
   <si>
     <t>Just Started</t>
+  </si>
+  <si>
+    <t>goalu lui iuli e sa fie o printesa</t>
+  </si>
+  <si>
+    <t>aNG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd/MM/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -134,17 +136,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,37 +452,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD17"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="1" max="1" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="10"/>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -502,7 +505,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -512,10 +515,10 @@
         <v>44241.456400462965</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -528,14 +531,14 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>44238.456400462965</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -552,10 +555,10 @@
         <v>44239.456400462965</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -566,16 +569,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>44236.456396574074</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -592,10 +595,10 @@
         <v>44236.456396574074</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -612,10 +615,10 @@
         <v>44236.456396574074</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -632,10 +635,10 @@
         <v>44237.647051111111</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -649,13 +652,13 @@
         <v>18</v>
       </c>
       <c r="C10" s="4">
-        <v>44238.650255671295</v>
+        <v>44239.650395219905</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -669,13 +672,13 @@
         <v>19</v>
       </c>
       <c r="C11" s="5">
-        <v>44239.650395219905</v>
+        <v>44247.652703865744</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -686,42 +689,68 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="6">
-        <v>44247.652703865744</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="7">
+        <v>44237.720787835649</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="8">
+        <v>36211.811375428239</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="n" s="9">
-        <v>44237.72078783565</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="9">
+        <v>44237.853477129633</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge scierea & citirea goalurilor + taskurilor din Excelgit add .!
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Task2.2</t>
   </si>
   <si>
-    <t>Task2.n</t>
-  </si>
-  <si>
     <t>Estimated Date</t>
   </si>
   <si>
@@ -58,48 +55,64 @@
     <t>do the model</t>
   </si>
   <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>0|0</t>
+  </si>
+  <si>
+    <t>Task2.3</t>
+  </si>
+  <si>
+    <t>do the finsish</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>aba</t>
+  </si>
+  <si>
+    <t>1|1</t>
+  </si>
+  <si>
+    <t>Just Started</t>
+  </si>
+  <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>fafsafa</t>
-  </si>
-  <si>
-    <t>abc2</t>
-  </si>
-  <si>
-    <t>VREAU SA FIU ARTIST</t>
-  </si>
-  <si>
-    <t>0|0</t>
-  </si>
-  <si>
-    <t>finish this damn app</t>
-  </si>
-  <si>
-    <t>brandNewGoal -&gt; IULI CONDUCE LUMEEEEA</t>
-  </si>
-  <si>
-    <t>Just Started</t>
-  </si>
-  <si>
-    <t>goalu lui iuli e sa fie o printesa</t>
-  </si>
-  <si>
-    <t>aNG</t>
+    <t>newGoal</t>
+  </si>
+  <si>
+    <t>gsaga</t>
+  </si>
+  <si>
+    <t>2|2</t>
+  </si>
+  <si>
+    <t>FINISHHHHH</t>
+  </si>
+  <si>
+    <t>5|5</t>
+  </si>
+  <si>
+    <t>hopa</t>
+  </si>
+  <si>
+    <t>4|4</t>
+  </si>
+  <si>
+    <t>anotherGoal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/MM/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -136,18 +149,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,44 +467,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A7" sqref="A7:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="6"/>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -498,30 +513,30 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>44241.456400462965</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -529,19 +544,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
         <v>44238.456400462965</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -549,208 +564,177 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>44239.456400462965</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5">
+        <v>44239.456400462965</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="n" s="7">
+        <v>44244.52785605324</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="n" s="10">
+        <v>44247.52857141204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="n" s="8">
+        <v>44239.52817125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="n" s="9">
+        <v>44246.52831228009</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="n" s="11">
+        <v>44247.52876335648</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="n" s="12">
+        <v>44246.52899694444</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2">
-        <v>44236.456396574074</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3">
-        <v>44237.647051111111</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4">
-        <v>44239.650395219905</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5">
-        <v>44247.652703865744</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7">
-        <v>44237.720787835649</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="8">
-        <v>36211.811375428239</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="9">
-        <v>44237.853477129633</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
little GUI bug ??-> Delete Task. TODO: deleteTaskRow in Excel
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>anotherGoal</t>
+  </si>
+  <si>
+    <t>uguigiuhiuh</t>
+  </si>
+  <si>
+    <t>guyguih9o</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -157,6 +163,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -467,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD15"/>
@@ -737,6 +746,75 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="n" s="13">
+        <v>44247.64841393519</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="n" s="14">
+        <v>44239.74582532408</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="n" s="15">
+        <v>44238.746113761576</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
functioneaza si DELETE TASK (interf+Excel)
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -85,9 +85,6 @@
     <t>newGoal</t>
   </si>
   <si>
-    <t>gsaga</t>
-  </si>
-  <si>
     <t>2|2</t>
   </si>
   <si>
@@ -97,19 +94,25 @@
     <t>5|5</t>
   </si>
   <si>
-    <t>hopa</t>
-  </si>
-  <si>
-    <t>4|4</t>
-  </si>
-  <si>
-    <t>anotherGoal</t>
-  </si>
-  <si>
     <t>uguigiuhiuh</t>
   </si>
   <si>
     <t>guyguih9o</t>
+  </si>
+  <si>
+    <t>brandNewGoal</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>noDelete</t>
+  </si>
+  <si>
+    <t>aTaskBecauseTheOtherWasDeleted</t>
+  </si>
+  <si>
+    <t>2|30</t>
   </si>
 </sst>
 </file>
@@ -155,22 +158,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -476,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,20 +494,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="12"/>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -550,13 +551,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>44238.456400462965</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44239.456400462965</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -570,12 +571,12 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5">
         <v>44239.456400462965</v>
       </c>
       <c r="D5" t="s">
@@ -590,16 +591,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5">
-        <v>44239.456400462965</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44244.527856053239</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -607,19 +608,22 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="n" s="7">
-        <v>44244.52785605324</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="8">
+        <v>44247.52857141204</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -631,18 +635,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="n" s="10">
-        <v>44247.52857141204</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="7">
+        <v>44239.52817125</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -656,16 +660,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="n" s="8">
-        <v>44239.52817125</v>
+        <v>31</v>
+      </c>
+      <c r="C9" t="n" s="13">
+        <v>44246.84532611111</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -677,18 +681,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="n" s="9">
-        <v>44246.52831228009</v>
+        <v>26</v>
+      </c>
+      <c r="C10" s="9">
+        <v>44239.745825324077</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -700,18 +704,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="n" s="11">
-        <v>44247.52876335648</v>
+      <c r="C11" s="10">
+        <v>44238.746113761576</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -723,15 +727,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="n" s="12">
-        <v>44246.52899694444</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="11">
+        <v>44238.814390023152</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -743,75 +747,6 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="n" s="13">
-        <v>44247.64841393519</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="n" s="14">
-        <v>44239.74582532408</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="n" s="15">
-        <v>44238.746113761576</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
totul functioneaza. trebuie sa aranjez codul si sa schimb culorile
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Goal2</t>
   </si>
   <si>
-    <t>Task2.1</t>
-  </si>
-  <si>
     <t>Task2.2</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>I will make StandApp in 2 months</t>
   </si>
   <si>
-    <t>do the view</t>
-  </si>
-  <si>
     <t>do the model</t>
   </si>
   <si>
@@ -103,16 +97,49 @@
     <t>brandNewGoal</t>
   </si>
   <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>noDelete</t>
-  </si>
-  <si>
     <t>aTaskBecauseTheOtherWasDeleted</t>
   </si>
   <si>
     <t>2|30</t>
+  </si>
+  <si>
+    <t>1|3</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>Something Done</t>
+  </si>
+  <si>
+    <t>aNewTaskForANewGoal</t>
+  </si>
+  <si>
+    <t>2|3</t>
+  </si>
+  <si>
+    <t>anotherTask</t>
+  </si>
+  <si>
+    <t>4|6</t>
+  </si>
+  <si>
+    <t>nTask</t>
+  </si>
+  <si>
+    <t>5|6</t>
+  </si>
+  <si>
+    <t>80%</t>
+  </si>
+  <si>
+    <t>Almost Done</t>
+  </si>
+  <si>
+    <t>15%</t>
   </si>
 </sst>
 </file>
@@ -158,10 +185,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -171,7 +197,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -477,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -523,231 +552,263 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>44241.456400462965</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>44239.456400462965</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4">
         <v>44239.456400462965</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44239.52817125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6">
-        <v>44244.527856053239</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8">
-        <v>44247.52857141204</v>
+        <v>27</v>
+      </c>
+      <c r="C7" s="11">
+        <v>44246.845326111114</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8">
+        <v>44239.745825324077</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9">
+        <v>44238.746113761576</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="7">
-        <v>44239.52817125</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="n" s="13">
-        <v>44246.84532611111</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="9">
-        <v>44239.745825324077</v>
+      <c r="C10" s="10">
+        <v>44238.814390023152</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="10">
-        <v>44238.746113761576</v>
+        <v>33</v>
+      </c>
+      <c r="C11" t="n" s="13">
+        <v>43874.49643962963</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="11">
-        <v>44238.814390023152</v>
+        <v>35</v>
+      </c>
+      <c r="C12" t="n" s="14">
+        <v>44253.51310829861</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="n" s="15">
+        <v>44233.51383005787</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>